<commit_message>
Remove gooyey | add user settings
</commit_message>
<xml_diff>
--- a/settings/users.xlsx
+++ b/settings/users.xlsx
@@ -11,18 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>Имя пользователя</t>
   </si>
   <si>
     <t>Чат ID</t>
-  </si>
-  <si>
-    <t>Иван Ковалев</t>
-  </si>
-  <si>
-    <t>Дмитрий</t>
   </si>
 </sst>
 </file>
@@ -69,7 +63,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -92,13 +86,113 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -108,19 +202,46 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -141,6 +262,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -339,17 +461,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -376,10 +498,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -618,12 +740,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -900,7 +1022,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -927,10 +1049,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1172,15 +1294,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.5781" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6719" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1190,46 +1313,72 @@
       <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>83256012</v>
-      </c>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1421555600</v>
-      </c>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>